<commit_message>
checkpoint on field-mapping work
</commit_message>
<xml_diff>
--- a/web/templates/grdi_1m/exampleInput/GRDI_Test_Bad_Metadata.xlsx
+++ b/web/templates/grdi_1m/exampleInput/GRDI_Test_Bad_Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damion/Documents/GitHub/DataHarmonizer/web/templates/grdi_1m/exampleInput/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8D34C-0A49-2441-A7F4-4EA44406AB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742E0726-C902-B149-A5A5-3A09222EBB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2180" windowWidth="21740" windowHeight="19680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7640" yWindow="1340" windowWidth="21740" windowHeight="19680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRDISamples" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="348">
   <si>
     <t>Sample collection and processing</t>
   </si>
@@ -1108,25 +1108,22 @@
   </si>
   <si>
     <t>progny_isolate_ID</t>
+  </si>
+  <si>
+    <t>EXAMPLE EXTRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -5235,15 +5232,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>234</v>
       </c>
@@ -5251,7 +5255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5283,13 +5287,16 @@
         <v>242</v>
       </c>
       <c r="K2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L2" t="s">
         <v>243</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -5320,14 +5327,14 @@
       <c r="J3" t="s">
         <v>184</v>
       </c>
-      <c r="K3" t="s">
-        <v>184</v>
-      </c>
       <c r="L3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>207</v>
       </c>
@@ -5358,14 +5365,14 @@
       <c r="J4" t="s">
         <v>184</v>
       </c>
-      <c r="K4" t="s">
-        <v>184</v>
-      </c>
       <c r="L4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -5396,14 +5403,14 @@
       <c r="J5" t="s">
         <v>184</v>
       </c>
-      <c r="K5" t="s">
-        <v>184</v>
-      </c>
       <c r="L5" t="s">
+        <v>184</v>
+      </c>
+      <c r="M5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>223</v>
       </c>
@@ -5434,14 +5441,14 @@
       <c r="J6" t="s">
         <v>184</v>
       </c>
-      <c r="K6" t="s">
-        <v>184</v>
-      </c>
       <c r="L6" t="s">
+        <v>184</v>
+      </c>
+      <c r="M6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -5472,17 +5479,17 @@
       <c r="J7" t="s">
         <v>184</v>
       </c>
-      <c r="K7" t="s">
-        <v>184</v>
-      </c>
       <c r="L7" t="s">
+        <v>184</v>
+      </c>
+      <c r="M7" t="s">
         <v>255</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="H1:H7 A1:F1 I1:L7 A3:F7 A2:C2 E2:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 L1:M7 A3:F7 A2:C2 E2:F2 H1:J7" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>